<commit_message>
fix bug other class
</commit_message>
<xml_diff>
--- a/pca_result.xlsx
+++ b/pca_result.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
   <si>
     <t>acc_train_before</t>
   </si>
@@ -81,6 +82,15 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>prior=0.01 other</t>
+  </si>
+  <si>
+    <t>prior=0.001 other</t>
   </si>
 </sst>
 </file>
@@ -185,7 +195,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -431,11 +440,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="413986696"/>
-        <c:axId val="413987088"/>
+        <c:axId val="102889208"/>
+        <c:axId val="102889992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="413986696"/>
+        <c:axId val="102889208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -477,7 +486,7 @@
             <a:endParaRPr lang="th-TH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413987088"/>
+        <c:crossAx val="102889992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -485,7 +494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="413987088"/>
+        <c:axId val="102889992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +545,7 @@
             <a:endParaRPr lang="th-TH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413986696"/>
+        <c:crossAx val="102889208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -550,7 +559,570 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="th-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="th-TH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Compare</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> prior</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40393744531933506"/>
+          <c:y val="4.1666666666666664E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="th-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prior=0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$17:$M$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-2.8921568626999961E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.10909090909100005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.19514237855900002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4159592530000022E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5834767642000092E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.4246100520000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8508771920000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.21031746031799997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.18204099821700004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.36379928315400001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.1070713461122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prior=0.001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$17:$N$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6.5359477100002117E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.2281639900001426E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.3077837200000692E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prior=0.01 other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$17:$O$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-4.5523697551146991E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.5233241953055012E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.6049119501189968E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27395338330906505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2282532231796095E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.29620325196569408</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.31184711528270598</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0999272242951976E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.6693807653518946E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15373846365203903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.96505263400991E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prior=0.001 other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$17:$P$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.6713321293513974E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18273550815934603</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.13092694364140001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30093674037831097</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.15802814295702494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.50818218490427602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.9199533336263812E-13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.5432098769949665E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9496184101039944E-13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.120071684709012E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.5717483986391298E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="102885288"/>
+        <c:axId val="102886072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="102885288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="th-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="102886072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="102886072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="th-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="102885288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -657,7 +1229,560 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1200,6 +2325,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1471,18 +2626,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="14" max="14" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1490,7 +2646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +2684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1570,7 +2726,7 @@
         <v>-0.10816993463999997</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1612,7 +2768,7 @@
         <v>-0.301487603306</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1654,7 +2810,7 @@
         <v>-0.31876046901100002</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1696,7 +2852,7 @@
         <v>6.044142614600001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1738,7 +2894,7 @@
         <v>-0.15249569707399996</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1780,7 +2936,7 @@
         <v>-0.48613518197600003</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1822,7 +2978,7 @@
         <v>2.0394736841999994E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1864,7 +3020,7 @@
         <v>-9.5238095238999954E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1906,7 +3062,7 @@
         <v>-0.14483065953600005</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1948,7 +3104,7 @@
         <v>7.6612903226000006E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" ref="B13:J13" si="1">AVERAGE(B3:B12)</f>
         <v>0.98589055510839996</v>
@@ -1993,21 +3149,21 @@
         <v>-0.31392143311800014</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" ref="N13:O13" si="2">SUM(N3:N12)</f>
+        <f>SUM(N3:N12)</f>
         <v>-1.571949927700006E-2</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="2"/>
+        <f>SUM(O3:O12)</f>
         <v>-1.4496685745680002</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2015,7 +3171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -2043,8 +3199,20 @@
       <c r="J16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2076,8 +3244,20 @@
         <f>I17-G17</f>
         <v>9.6405228759999795E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>-2.8921568626999961E-2</v>
+      </c>
+      <c r="N17">
+        <v>6.5359477100002117E-4</v>
+      </c>
+      <c r="O17">
+        <v>-4.5523697551146991E-2</v>
+      </c>
+      <c r="P17">
+        <v>5.6713321293513974E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2106,11 +3286,23 @@
         <v>0.46727272727300001</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:J26" si="3">I18-G18</f>
+        <f t="shared" ref="J18:J26" si="2">I18-G18</f>
         <v>-0.158181818182</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>-0.10909090909100005</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>-5.5233241953055012E-2</v>
+      </c>
+      <c r="P18">
+        <v>0.18273550815934603</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2139,11 +3331,23 @@
         <v>0.52797319932999998</v>
       </c>
       <c r="J19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-9.9832495812000044E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>-0.19514237855900002</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>-6.6049119501189968E-2</v>
+      </c>
+      <c r="P19">
+        <v>-0.13092694364140001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2172,11 +3376,23 @@
         <v>0.26926994906599999</v>
       </c>
       <c r="J20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.0050933785999989E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>5.4159592530000022E-2</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0.27395338330906505</v>
+      </c>
+      <c r="P20">
+        <v>0.30093674037831097</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2205,11 +3421,23 @@
         <v>0.65352839931200002</v>
       </c>
       <c r="J21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.10499139414800007</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>1.5834767642000092E-2</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1.2282532231796095E-2</v>
+      </c>
+      <c r="P21">
+        <v>-0.15802814295702494</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2238,11 +3466,23 @@
         <v>0.78370883882099995</v>
       </c>
       <c r="J22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-4.8180242635000092E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>-5.4246100520000007E-2</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>-0.29620325196569408</v>
+      </c>
+      <c r="P22">
+        <v>-0.50818218490427602</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2271,11 +3511,23 @@
         <v>0.41184210526300002</v>
       </c>
       <c r="J23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.14451754385900001</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>2.8508771920000009E-3</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0.31184711528270598</v>
+      </c>
+      <c r="P23">
+        <v>-4.9199533336263812E-13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7</v>
       </c>
@@ -2304,11 +3556,23 @@
         <v>0.23633156966499999</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.27050264550299996</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>-0.21031746031799997</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>5.0999272242951976E-2</v>
+      </c>
+      <c r="P24">
+        <v>-1.5432098769949665E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2337,11 +3601,23 @@
         <v>0.66867201426</v>
       </c>
       <c r="J25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.19942067736199998</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>-0.18204099821700004</v>
+      </c>
+      <c r="N25">
+        <v>-2.2281639900001426E-4</v>
+      </c>
+      <c r="O25">
+        <v>5.6693807653518946E-2</v>
+      </c>
+      <c r="P25">
+        <v>3.9496184101039944E-13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2370,49 +3646,94 @@
         <v>0.43615591397800002</v>
       </c>
       <c r="J26">
+        <f t="shared" si="2"/>
+        <v>7.2356630824000012E-2</v>
+      </c>
+      <c r="M26">
+        <v>-0.36379928315400001</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0.15373846365203903</v>
+      </c>
+      <c r="P26">
+        <v>1.120071684709012E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <f t="shared" ref="B27:J27" si="3">AVERAGE(B17:B26)</f>
+        <v>0.98589055510839996</v>
+      </c>
+      <c r="C27">
         <f t="shared" si="3"/>
-        <v>7.2356630824000012E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B27">
-        <f t="shared" ref="B27" si="4">AVERAGE(B17:B26)</f>
-        <v>0.98589055510839996</v>
-      </c>
-      <c r="C27">
-        <f t="shared" ref="C27" si="5">AVERAGE(C17:C26)</f>
         <v>0.1681133083961</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27" si="6">AVERAGE(D17:D26)</f>
+        <f t="shared" si="3"/>
         <v>0.93332144173300002</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27" si="7">AVERAGE(E17:E26)</f>
+        <f t="shared" si="3"/>
         <v>0.15856661283840001</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27" si="8">AVERAGE(F17:F26)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="G27" si="9">AVERAGE(G17:G26)</f>
+        <f t="shared" si="3"/>
         <v>0.49783173534999997</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27" si="10">AVERAGE(H17:H26)</f>
+        <f t="shared" si="3"/>
         <v>0.96879631770319996</v>
       </c>
       <c r="I27">
-        <f t="shared" ref="I27" si="11">AVERAGE(I17:I26)</f>
+        <f t="shared" si="3"/>
         <v>0.49625978542230004</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27" si="12">AVERAGE(J17:J26)</f>
+        <f t="shared" si="3"/>
         <v>-1.571949927700006E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>-0.1070713461122</v>
+      </c>
+      <c r="N27">
+        <v>4.3077837200000692E-5</v>
+      </c>
+      <c r="O27">
+        <v>3.96505263400991E-2</v>
+      </c>
+      <c r="P27">
+        <v>-2.5717483986391298E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="1">
+        <f>AVERAGE(M17:M27)</f>
+        <v>-0.10707134611219998</v>
+      </c>
+      <c r="N28" s="1">
+        <f>AVERAGE(N17:N27)</f>
+        <v>4.3077837200000692E-5</v>
+      </c>
+      <c r="O28" s="1">
+        <f>AVERAGE(O17:O27)</f>
+        <v>3.96505263400991E-2</v>
+      </c>
+      <c r="P28" s="1">
+        <f>AVERAGE(P17:P27)</f>
+        <v>-2.5717483986391298E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2420,7 +3741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -2449,7 +3770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2482,7 +3803,7 @@
         <v>-0.10816993463999997</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2511,7 +3832,7 @@
         <v>0.32396694214900001</v>
       </c>
       <c r="J32">
-        <f t="shared" ref="J32:J40" si="13">I32-G32</f>
+        <f t="shared" ref="J32:J40" si="4">I32-G32</f>
         <v>-0.301487603306</v>
       </c>
     </row>
@@ -2544,7 +3865,7 @@
         <v>0.30904522613099999</v>
       </c>
       <c r="J33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-0.31876046901100002</v>
       </c>
     </row>
@@ -2577,7 +3898,7 @@
         <v>0.29966044142600001</v>
       </c>
       <c r="J34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>6.044142614600001E-2</v>
       </c>
     </row>
@@ -2610,7 +3931,7 @@
         <v>0.39604130808999999</v>
       </c>
       <c r="J35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-0.15249569707399996</v>
       </c>
     </row>
@@ -2643,7 +3964,7 @@
         <v>0.34575389948000002</v>
       </c>
       <c r="J36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-0.48613518197600003</v>
       </c>
     </row>
@@ -2676,7 +3997,7 @@
         <v>0.28771929824600001</v>
       </c>
       <c r="J37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>2.0394736841999994E-2</v>
       </c>
     </row>
@@ -2709,7 +4030,7 @@
         <v>0.41159611992900003</v>
       </c>
       <c r="J38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-9.5238095238999954E-2</v>
       </c>
     </row>
@@ -2742,7 +4063,7 @@
         <v>0.32442067736199998</v>
       </c>
       <c r="J39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-0.14483065953600005</v>
       </c>
     </row>
@@ -2775,45 +4096,45 @@
         <v>0.44041218638000001</v>
       </c>
       <c r="J40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>7.6612903226000006E-2</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B41">
-        <f t="shared" ref="B41" si="14">AVERAGE(B31:B40)</f>
+        <f t="shared" ref="B41:J41" si="5">AVERAGE(B31:B40)</f>
         <v>0.98589055510839996</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41" si="15">AVERAGE(C31:C40)</f>
+        <f t="shared" si="5"/>
         <v>0.1681133083961</v>
       </c>
       <c r="D41">
-        <f t="shared" ref="D41" si="16">AVERAGE(D31:D40)</f>
+        <f t="shared" si="5"/>
         <v>0.17943665645899998</v>
       </c>
       <c r="E41">
-        <f t="shared" ref="E41" si="17">AVERAGE(E31:E40)</f>
+        <f t="shared" si="5"/>
         <v>0.19145711450810005</v>
       </c>
       <c r="F41">
-        <f t="shared" ref="F41" si="18">AVERAGE(F31:F40)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G41">
-        <f t="shared" ref="G41" si="19">AVERAGE(G31:G40)</f>
+        <f t="shared" si="5"/>
         <v>0.49783173534999997</v>
       </c>
       <c r="H41">
-        <f t="shared" ref="H41" si="20">AVERAGE(H31:H40)</f>
+        <f t="shared" si="5"/>
         <v>0.48979472722360001</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I41" si="21">AVERAGE(I31:I40)</f>
+        <f t="shared" si="5"/>
         <v>0.35286487789319998</v>
       </c>
       <c r="J41">
-        <f t="shared" ref="J41" si="22">AVERAGE(J31:J40)</f>
+        <f t="shared" si="5"/>
         <v>-0.14496685745680002</v>
       </c>
     </row>
@@ -2916,7 +4237,7 @@
         <v>0.51636363636399996</v>
       </c>
       <c r="J46">
-        <f t="shared" ref="J46:J54" si="23">I46-G46</f>
+        <f t="shared" ref="J46:J54" si="6">I46-G46</f>
         <v>-0.10909090909100005</v>
       </c>
     </row>
@@ -2949,7 +4270,7 @@
         <v>0.432663316583</v>
       </c>
       <c r="J47">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>-0.19514237855900002</v>
       </c>
     </row>
@@ -2982,7 +4303,7 @@
         <v>0.29337860781000002</v>
       </c>
       <c r="J48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>5.4159592530000022E-2</v>
       </c>
     </row>
@@ -3015,7 +4336,7 @@
         <v>0.56437177280600004</v>
       </c>
       <c r="J49">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>1.5834767642000092E-2</v>
       </c>
     </row>
@@ -3048,7 +4369,7 @@
         <v>0.77764298093600004</v>
       </c>
       <c r="J50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>-5.4246100520000007E-2</v>
       </c>
     </row>
@@ -3081,7 +4402,7 @@
         <v>0.27017543859600002</v>
       </c>
       <c r="J51">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>2.8508771920000009E-3</v>
       </c>
     </row>
@@ -3114,7 +4435,7 @@
         <v>0.29651675485000001</v>
       </c>
       <c r="J52">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>-0.21031746031799997</v>
       </c>
     </row>
@@ -3147,7 +4468,7 @@
         <v>0.28721033868099999</v>
       </c>
       <c r="J53">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>-0.18204099821700004</v>
       </c>
     </row>
@@ -3168,45 +4489,45 @@
         <v>0.36379928315400001</v>
       </c>
       <c r="J54">
-        <f t="shared" si="23"/>
+        <f t="shared" si="6"/>
         <v>-0.36379928315400001</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B55">
-        <f t="shared" ref="B55" si="24">AVERAGE(B45:B54)</f>
+        <f t="shared" ref="B55:J55" si="7">AVERAGE(B45:B54)</f>
         <v>0.98589055510839996</v>
       </c>
       <c r="C55">
-        <f t="shared" ref="C55" si="25">AVERAGE(C45:C54)</f>
+        <f t="shared" si="7"/>
         <v>0.1681133083961</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55" si="26">AVERAGE(D45:D54)</f>
+        <f t="shared" si="7"/>
         <v>0.98307459683822218</v>
       </c>
       <c r="E55">
-        <f t="shared" ref="E55" si="27">AVERAGE(E45:E54)</f>
+        <f t="shared" si="7"/>
         <v>0.16091073001655556</v>
       </c>
       <c r="F55">
-        <f t="shared" ref="F55" si="28">AVERAGE(F45:F54)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G55">
-        <f t="shared" ref="G55" si="29">AVERAGE(G45:G54)</f>
+        <f t="shared" si="7"/>
         <v>0.49783173534999997</v>
       </c>
       <c r="H55">
-        <f t="shared" ref="H55" si="30">AVERAGE(H45:H54)</f>
+        <f t="shared" si="7"/>
         <v>0.99865827873966673</v>
       </c>
       <c r="I55">
-        <f t="shared" ref="I55" si="31">AVERAGE(I45:I54)</f>
+        <f t="shared" si="7"/>
         <v>0.43417821026422221</v>
       </c>
       <c r="J55">
-        <f t="shared" ref="J55" si="32">AVERAGE(J45:J54)</f>
+        <f t="shared" si="7"/>
         <v>-0.1070713461122</v>
       </c>
     </row>
@@ -3309,7 +4630,7 @@
         <v>0.62545454545500001</v>
       </c>
       <c r="J60">
-        <f t="shared" ref="J60:J68" si="33">I60-G60</f>
+        <f t="shared" ref="J60:J68" si="8">I60-G60</f>
         <v>0</v>
       </c>
     </row>
@@ -3342,7 +4663,7 @@
         <v>0.62780569514200002</v>
       </c>
       <c r="J61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3375,7 +4696,7 @@
         <v>0.23921901528</v>
       </c>
       <c r="J62">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3408,7 +4729,7 @@
         <v>0.54853700516399995</v>
       </c>
       <c r="J63">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3441,7 +4762,7 @@
         <v>0.83188908145600005</v>
       </c>
       <c r="J64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3474,7 +4795,7 @@
         <v>0.26732456140400002</v>
       </c>
       <c r="J65">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3507,7 +4828,7 @@
         <v>0.50683421516799998</v>
       </c>
       <c r="J66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3540,7 +4861,7 @@
         <v>0.46902852049900001</v>
       </c>
       <c r="J67">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>-2.2281639900001426E-4</v>
       </c>
     </row>
@@ -3573,46 +4894,917 @@
         <v>0.36379928315400001</v>
       </c>
       <c r="J68">
-        <f t="shared" si="33"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B69">
-        <f t="shared" ref="B69" si="34">AVERAGE(B59:B68)</f>
+        <f t="shared" ref="B69:J69" si="9">AVERAGE(B59:B68)</f>
         <v>0.98589055510839996</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69" si="35">AVERAGE(C59:C68)</f>
+        <f t="shared" si="9"/>
         <v>0.1681133083961</v>
       </c>
       <c r="D69">
-        <f t="shared" ref="D69" si="36">AVERAGE(D59:D68)</f>
+        <f t="shared" si="9"/>
         <v>0.98579647455139985</v>
       </c>
       <c r="E69">
-        <f t="shared" ref="E69" si="37">AVERAGE(E59:E68)</f>
+        <f t="shared" si="9"/>
         <v>0.16778288367350003</v>
       </c>
       <c r="F69">
-        <f t="shared" ref="F69" si="38">AVERAGE(F59:F68)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="G69">
-        <f t="shared" ref="G69" si="39">AVERAGE(G59:G68)</f>
+        <f t="shared" si="9"/>
         <v>0.49783173534999997</v>
       </c>
       <c r="H69">
-        <f t="shared" ref="H69" si="40">AVERAGE(H59:H68)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I69">
-        <f t="shared" ref="I69" si="41">AVERAGE(I59:I68)</f>
+        <f t="shared" si="9"/>
         <v>0.4978748131872</v>
       </c>
       <c r="J69">
-        <f t="shared" ref="J69" si="42">AVERAGE(J59:J68)</f>
+        <f t="shared" si="9"/>
         <v>4.3077837200000692E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
+        <v>3</v>
+      </c>
+      <c r="F72" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" t="s">
+        <v>5</v>
+      </c>
+      <c r="H72" t="s">
+        <v>6</v>
+      </c>
+      <c r="I72" t="s">
+        <v>7</v>
+      </c>
+      <c r="J72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <v>0.988372093023</v>
+      </c>
+      <c r="C73">
+        <v>0.18800648298200001</v>
+      </c>
+      <c r="D73">
+        <v>0.96797560045749098</v>
+      </c>
+      <c r="E73">
+        <v>0.18476499189627199</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>0.49820261437899999</v>
+      </c>
+      <c r="H73">
+        <v>0.94471631883577001</v>
+      </c>
+      <c r="I73">
+        <v>0.452678916827853</v>
+      </c>
+      <c r="J73">
+        <f>I73-G73</f>
+        <v>-4.5523697551146991E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>0.98629354654500001</v>
+      </c>
+      <c r="C74">
+        <v>0.175409836066</v>
+      </c>
+      <c r="D74">
+        <v>0.95907100704359405</v>
+      </c>
+      <c r="E74">
+        <v>0.17704918032786801</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>0.62545454545500001</v>
+      </c>
+      <c r="H74">
+        <v>0.927148880155785</v>
+      </c>
+      <c r="I74">
+        <v>0.570221303501945</v>
+      </c>
+      <c r="J74">
+        <f t="shared" ref="J74:J82" si="10">I74-G74</f>
+        <v>-5.5233241953055012E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="B75">
+        <v>0.98935563581099994</v>
+      </c>
+      <c r="C75">
+        <v>0.15614617940200001</v>
+      </c>
+      <c r="D75">
+        <v>0.96578597224862195</v>
+      </c>
+      <c r="E75">
+        <v>0.154485049833887</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0.62780569514200002</v>
+      </c>
+      <c r="H75">
+        <v>0.92909641235856899</v>
+      </c>
+      <c r="I75">
+        <v>0.56175657564081005</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="10"/>
+        <v>-6.6049119501189968E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>0.98861263997000004</v>
+      </c>
+      <c r="C76">
+        <v>0.181818181818</v>
+      </c>
+      <c r="D76">
+        <v>0.96128297589675404</v>
+      </c>
+      <c r="E76">
+        <v>0.17676767676767599</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>0.23921901528</v>
+      </c>
+      <c r="H76">
+        <v>0.93277849536388102</v>
+      </c>
+      <c r="I76">
+        <v>0.51317239858906505</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="10"/>
+        <v>0.27395338330906505</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>4</v>
+      </c>
+      <c r="B77">
+        <v>0.98806139852200003</v>
+      </c>
+      <c r="C77">
+        <v>0.175767918089</v>
+      </c>
+      <c r="D77">
+        <v>0.96399469395489801</v>
+      </c>
+      <c r="E77">
+        <v>0.15870307167235401</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>0.54853700516399995</v>
+      </c>
+      <c r="H77">
+        <v>0.94287468458027501</v>
+      </c>
+      <c r="I77">
+        <v>0.56081953739579604</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="10"/>
+        <v>1.2282532231796095E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>0.98769172505199998</v>
+      </c>
+      <c r="C78">
+        <v>0.14948453608199999</v>
+      </c>
+      <c r="D78">
+        <v>0.95815186517704898</v>
+      </c>
+      <c r="E78">
+        <v>0.14432989690721601</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>0.83188908145600005</v>
+      </c>
+      <c r="H78">
+        <v>0.931249762227366</v>
+      </c>
+      <c r="I78">
+        <v>0.53568582949030596</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="10"/>
+        <v>-0.29620325196569408</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>6</v>
+      </c>
+      <c r="B79">
+        <v>0.99168084704100001</v>
+      </c>
+      <c r="C79">
+        <v>0.17073170731699999</v>
+      </c>
+      <c r="D79">
+        <v>0.968992248062015</v>
+      </c>
+      <c r="E79">
+        <v>0.17770034843205501</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>0.26732456140400002</v>
+      </c>
+      <c r="H79">
+        <v>0.94015659631348003</v>
+      </c>
+      <c r="I79">
+        <v>0.57917167668670599</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="10"/>
+        <v>0.31184711528270598</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>7</v>
+      </c>
+      <c r="B80">
+        <v>0.98696145124699997</v>
+      </c>
+      <c r="C80">
+        <v>0.18388791593699999</v>
+      </c>
+      <c r="D80">
+        <v>0.96012849584278104</v>
+      </c>
+      <c r="E80">
+        <v>0.194395796847635</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>0.50683421516799998</v>
+      </c>
+      <c r="H80">
+        <v>0.92846083936136703</v>
+      </c>
+      <c r="I80">
+        <v>0.55783348741095196</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="10"/>
+        <v>5.0999272242951976E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>8</v>
+      </c>
+      <c r="B81">
+        <v>0.96526991317499999</v>
+      </c>
+      <c r="C81">
+        <v>0.155752212389</v>
+      </c>
+      <c r="D81">
+        <v>0.91072102680256695</v>
+      </c>
+      <c r="E81">
+        <v>0.19115044247787599</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>0.46925133689800003</v>
+      </c>
+      <c r="H81">
+        <v>0.89483759136322005</v>
+      </c>
+      <c r="I81">
+        <v>0.52594514455151897</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="10"/>
+        <v>5.6693807653518946E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>9</v>
+      </c>
+      <c r="B82">
+        <v>0.98660630069800004</v>
+      </c>
+      <c r="C82">
+        <v>0.14412811387900001</v>
+      </c>
+      <c r="D82">
+        <v>0.95642331635540401</v>
+      </c>
+      <c r="E82">
+        <v>0.15658362989323801</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0.36379928315400001</v>
+      </c>
+      <c r="H82">
+        <v>0.93380315188616803</v>
+      </c>
+      <c r="I82">
+        <v>0.51753774680603903</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="10"/>
+        <v>0.15373846365203903</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <f t="shared" ref="B83:J83" si="11">AVERAGE(B73:B82)</f>
+        <v>0.98589055510839996</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="11"/>
+        <v>0.1681133083961</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="11"/>
+        <v>0.95725272018411744</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="11"/>
+        <v>0.17159300850560771</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="11"/>
+        <v>0.49783173534999997</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="11"/>
+        <v>0.93051227324458829</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="11"/>
+        <v>0.53748226169009905</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="11"/>
+        <v>3.96505263400991E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>3</v>
+      </c>
+      <c r="F86" t="s">
+        <v>4</v>
+      </c>
+      <c r="G86" t="s">
+        <v>5</v>
+      </c>
+      <c r="H86" t="s">
+        <v>6</v>
+      </c>
+      <c r="I86" t="s">
+        <v>7</v>
+      </c>
+      <c r="J86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>0</v>
+      </c>
+      <c r="B87">
+        <v>0.988372093023</v>
+      </c>
+      <c r="C87">
+        <v>0.18800648298200001</v>
+      </c>
+      <c r="D87">
+        <v>0.98856271444910404</v>
+      </c>
+      <c r="E87">
+        <v>0.18638573743922199</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>0.49820261437899999</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>0.55491593567251396</v>
+      </c>
+      <c r="J87">
+        <f>I87-G87</f>
+        <v>5.6713321293513974E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>0.98629354654500001</v>
+      </c>
+      <c r="C88">
+        <v>0.175409836066</v>
+      </c>
+      <c r="D88">
+        <v>0.98629354654483103</v>
+      </c>
+      <c r="E88">
+        <v>0.173770491803278</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>0.62545454545500001</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>0.80819005361434604</v>
+      </c>
+      <c r="J88">
+        <f t="shared" ref="J88:J96" si="12">I88-G88</f>
+        <v>0.18273550815934603</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>2</v>
+      </c>
+      <c r="B89">
+        <v>0.98935563581099994</v>
+      </c>
+      <c r="C89">
+        <v>0.15614617940200001</v>
+      </c>
+      <c r="D89">
+        <v>0.98935563581068198</v>
+      </c>
+      <c r="E89">
+        <v>0.15780730897009901</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>0.62780569514200002</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>0.49687875150060001</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="12"/>
+        <v>-0.13092694364140001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>3</v>
+      </c>
+      <c r="B90">
+        <v>0.98861263997000004</v>
+      </c>
+      <c r="C90">
+        <v>0.181818181818</v>
+      </c>
+      <c r="D90">
+        <v>0.98880242930347295</v>
+      </c>
+      <c r="E90">
+        <v>0.18013468013468001</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>0.23921901528</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
+        <v>0.54015575565831098</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="12"/>
+        <v>0.30093674037831097</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>4</v>
+      </c>
+      <c r="B91">
+        <v>0.98806139852200003</v>
+      </c>
+      <c r="C91">
+        <v>0.175767918089</v>
+      </c>
+      <c r="D91">
+        <v>0.98806139852188701</v>
+      </c>
+      <c r="E91">
+        <v>0.17747440273037501</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>0.54853700516399995</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>0.390508862206975</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="12"/>
+        <v>-0.15802814295702494</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>0.98769172505199998</v>
+      </c>
+      <c r="C92">
+        <v>0.14948453608199999</v>
+      </c>
+      <c r="D92">
+        <v>0.98769172505207303</v>
+      </c>
+      <c r="E92">
+        <v>0.149484536082474</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>0.83188908145600005</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>0.32370689655172402</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="12"/>
+        <v>-0.50818218490427602</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>6</v>
+      </c>
+      <c r="B93">
+        <v>0.99168084704100001</v>
+      </c>
+      <c r="C93">
+        <v>0.17073170731699999</v>
+      </c>
+      <c r="D93">
+        <v>0.99168084704102799</v>
+      </c>
+      <c r="E93">
+        <v>0.17073170731707299</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93">
+        <v>0.26732456140400002</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>0.26732456140350802</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="12"/>
+        <v>-4.9199533336263812E-13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>7</v>
+      </c>
+      <c r="B94">
+        <v>0.98696145124699997</v>
+      </c>
+      <c r="C94">
+        <v>0.18388791593699999</v>
+      </c>
+      <c r="D94">
+        <v>0.98696145124716494</v>
+      </c>
+      <c r="E94">
+        <v>0.18038528896672501</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>0.50683421516799998</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>0.50529100529100501</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="12"/>
+        <v>-1.5432098769949665E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>8</v>
+      </c>
+      <c r="B95">
+        <v>0.96526991317499999</v>
+      </c>
+      <c r="C95">
+        <v>0.155752212389</v>
+      </c>
+      <c r="D95">
+        <v>0.96526991317478295</v>
+      </c>
+      <c r="E95">
+        <v>0.15575221238938</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95">
+        <v>0.46925133689800003</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>0.46925133689839499</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="12"/>
+        <v>3.9496184101039944E-13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>9</v>
+      </c>
+      <c r="B96">
+        <v>0.98660630069800004</v>
+      </c>
+      <c r="C96">
+        <v>0.14412811387900001</v>
+      </c>
+      <c r="D96">
+        <v>0.98660630069798105</v>
+      </c>
+      <c r="E96">
+        <v>0.14412811387900301</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96">
+        <v>0.36379928315400001</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>0.36491935483870902</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="12"/>
+        <v>1.120071684709012E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <f t="shared" ref="B97:J97" si="13">AVERAGE(B87:B96)</f>
+        <v>0.98589055510839996</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="13"/>
+        <v>0.1681133083961</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="13"/>
+        <v>0.98592859618430073</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="13"/>
+        <v>0.16760544797123086</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="13"/>
+        <v>0.49783173534999997</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="13"/>
+        <v>0.47211425136360868</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="13"/>
+        <v>-2.5717483986391298E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D115">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D119">
+        <v>0.999999999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D124">
+        <v>0.999999999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D130">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>